<commit_message>
ajout du plan ip
</commit_message>
<xml_diff>
--- a/planIP/Plan_Adressage_ip.xlsx
+++ b/planIP/Plan_Adressage_ip.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxou\Documents\projet_b3infra\git\infraProjetIntranet\planIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\travail\Ynov\Projet B3\github\infraProjetIntranet\planIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392EED5-6AB1-47B3-BCAD-D930E69069E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95757B41-57D7-4C85-A9FF-A973527C5C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA5A4537-08DC-4692-B4CA-66169E76DEED}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{BA5A4537-08DC-4692-B4CA-66169E76DEED}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>PLAN d'adressage IP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Hostname</t>
   </si>
@@ -79,42 +76,57 @@
 Intranet</t>
   </si>
   <si>
-    <t>lan : 10
-OPT1: 20
-OPT2: 99</t>
+    <t>192.168.10.10</t>
+  </si>
+  <si>
+    <t>192.168.99.99</t>
+  </si>
+  <si>
+    <t>Tnas</t>
+  </si>
+  <si>
+    <t>NAS</t>
+  </si>
+  <si>
+    <t>192.168.1.78</t>
+  </si>
+  <si>
+    <t>srvmail</t>
+  </si>
+  <si>
+    <t>server-AD</t>
+  </si>
+  <si>
+    <t>192.168.10.5</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>réseau</t>
   </si>
   <si>
     <t>WAN : 192.168.1.99
 LAN : 192.168.10.1
-OPT1 : 192.168.20.1
-OPT2 : 192.168.99.1</t>
-  </si>
-  <si>
-    <t>192.168.10.10</t>
-  </si>
-  <si>
-    <t>192.168.99.99</t>
-  </si>
-  <si>
-    <t>Tnas</t>
-  </si>
-  <si>
-    <t>NAS</t>
-  </si>
-  <si>
-    <t>192.168.1.78</t>
-  </si>
-  <si>
-    <t>srvmail</t>
-  </si>
-  <si>
-    <t>server-AD</t>
-  </si>
-  <si>
-    <t>192.168.10.5</t>
-  </si>
-  <si>
-    <t>Mail</t>
+WEB : 192.168.99.1</t>
+  </si>
+  <si>
+    <t>lan :10
+OPT2: 99</t>
+  </si>
+  <si>
+    <t>WAN : 192.168.1.0/24
+LAN : 192.168.10.0/24
+WEB : 192.168.99.0/24</t>
+  </si>
+  <si>
+    <t>192.168.10.0/24</t>
+  </si>
+  <si>
+    <t>192.168.99.0/24</t>
+  </si>
+  <si>
+    <t>192.168.1.0/24</t>
   </si>
 </sst>
 </file>
@@ -165,7 +177,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -189,12 +204,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD19F291-5C7B-4668-BB46-EE421C5F3951}" name="Tableau1" displayName="Tableau1" ref="A5:E10" totalsRowShown="0">
-  <autoFilter ref="A5:E10" xr:uid="{FD19F291-5C7B-4668-BB46-EE421C5F3951}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{20605D50-BD47-4A88-AC58-78F29611A216}" name="Hostname" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{423F87AA-B641-4015-8B65-74E0DB0B734E}" name="Device" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{F1BD2519-762A-4FF3-99C8-1AEBAB380830}" name="IP" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD19F291-5C7B-4668-BB46-EE421C5F3951}" name="Tableau1" displayName="Tableau1" ref="A1:F6" totalsRowShown="0">
+  <autoFilter ref="A1:F6" xr:uid="{FD19F291-5C7B-4668-BB46-EE421C5F3951}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{20605D50-BD47-4A88-AC58-78F29611A216}" name="Hostname" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{423F87AA-B641-4015-8B65-74E0DB0B734E}" name="Device" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F1BD2519-762A-4FF3-99C8-1AEBAB380830}" name="IP" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{51F9A4B2-36EF-4CDE-8B2B-A0FC9C9FF13D}" name="réseau" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{EF93F5B3-42D5-4CE3-A7DC-D1A24898DA03}" name="LAN"/>
     <tableColumn id="5" xr3:uid="{9187AAD2-4385-43D8-AE4C-5BBDAC9EFC39}" name="Commentaire"/>
   </tableColumns>
@@ -499,117 +515,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E491F89-0EFE-40BB-9804-8E74628C1E13}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>99</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>99</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>